<commit_message>
GST Input data ready
</commit_message>
<xml_diff>
--- a/docs/gst-summary.xlsx
+++ b/docs/gst-summary.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Projects\dotnet\Prints\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C38CBC0-7EE9-4CDA-A111-EC3CC8A383EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD35E79-8083-4053-A1BD-B32F3DF7D642}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{7280A6F5-D76D-4628-A60A-3757CA53AC55}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{7280A6F5-D76D-4628-A60A-3757CA53AC55}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GSTInput-Cols" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -523,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{900E4611-3E2E-4B1A-AB9B-1C314BB932C7}">
   <dimension ref="B3:Q8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -640,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C1B75F-6681-44C8-B5DC-0AC4ACF765F4}">
   <dimension ref="B1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>